<commit_message>
Changes to data and API-scripts to force uncached runs
*Dummy parameter toegevoegd waarmee d.m.v. een random-getal uncached API-runs kunnen worden geforceerd zonder modelinstellingen aan te passen.
-Mogelijke bug: bij het 1000-agents experiment loopt de cloud vast, maar het offline model werkt gewoon..
</commit_message>
<xml_diff>
--- a/Base/APIOutputAgentData_default.xlsx
+++ b/Base/APIOutputAgentData_default.xlsx
@@ -531,7 +531,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>hh13</t>
+          <t>hh1</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -551,7 +551,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[12]</t>
+          <t>root.pop_gridConnections[0]</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -561,7 +561,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>0.252</t>
+          <t>0.3</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -571,7 +571,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>0.5020286982281488</t>
+          <t>0.602017313814645</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -601,7 +601,7 @@
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>-218.26944423211674</t>
+          <t>-554.9071135646353</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
@@ -611,7 +611,7 @@
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>-207.25320797397367</t>
+          <t>-207.2880356929771</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
@@ -626,7 +626,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>hh14</t>
+          <t>hh2</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -646,7 +646,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[13]</t>
+          <t>root.pop_gridConnections[1]</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -656,7 +656,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>0.252</t>
+          <t>0.3</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -666,7 +666,7 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>0.5020286982281488</t>
+          <t>0.602017313814645</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -696,7 +696,7 @@
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>-500.2994442320691</t>
+          <t>-227.6011135646638</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
@@ -706,7 +706,7 @@
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>-207.25320797397367</t>
+          <t>-207.2880356929771</t>
         </is>
       </c>
       <c r="S3" t="inlineStr">
@@ -721,7 +721,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>hh15</t>
+          <t>hh3</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -741,27 +741,27 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[14]</t>
+          <t>root.pop_gridConnections[2]</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>null</t>
+          <t>root.pop_energySuppliers[1]</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>0.252</t>
+          <t>0.3</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.5776933819433462</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>0.5020286982281488</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -791,17 +791,17 @@
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>-431.2934442320796</t>
+          <t>-163.71911356467206</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-397.82552304712624</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>-207.25320797397367</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="S4" t="inlineStr">
@@ -816,7 +816,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>hh1</t>
+          <t>hh4</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -826,17 +826,17 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>sup1</t>
+          <t>hol1</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[0]</t>
+          <t>root.pop_energyHolons[0]( p_actorID = hol1, p_actorType = holon, p_parentActorID = sup2 )</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[0]</t>
+          <t>root.pop_gridConnections[3]</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -846,7 +846,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>0.252</t>
+          <t>0.3</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -856,7 +856,7 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>0.5020286982281488</t>
+          <t>0.602017313814645</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
@@ -886,7 +886,7 @@
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>-554.8574442320602</t>
+          <t>-797.4991135646349</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr">
@@ -896,7 +896,7 @@
       </c>
       <c r="R5" t="inlineStr">
         <is>
-          <t>-207.25320797397367</t>
+          <t>-207.2880356929771</t>
         </is>
       </c>
       <c r="S5" t="inlineStr">
@@ -911,7 +911,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>hh11</t>
+          <t>hh5</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -921,37 +921,37 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>hol1</t>
+          <t>sup1</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>root.pop_energyHolons[0]( p_actorID = hol1, p_actorType = holon, p_parentActorID = sup2 )</t>
+          <t>root.pop_energySuppliers[0]</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[10]</t>
+          <t>root.pop_gridConnections[4]</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>null</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>0.252</t>
+          <t>0.3</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>0.4817447104209508</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.602017313814645</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
@@ -981,17 +981,17 @@
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>-135.2774442321169</t>
+          <t>-186.1471135646692</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>-397.75868197025045</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-207.2880356929771</t>
         </is>
       </c>
       <c r="S6" t="inlineStr">
@@ -1006,7 +1006,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>hh2</t>
+          <t>hh6</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -1026,7 +1026,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[1]</t>
+          <t>root.pop_gridConnections[5]</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -1036,7 +1036,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>0.252</t>
+          <t>0.3</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -1046,7 +1046,7 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>0.5020286982281488</t>
+          <t>0.602017313814645</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
@@ -1076,7 +1076,7 @@
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>-227.55144423211712</t>
+          <t>-1164.831113564687</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
@@ -1086,7 +1086,7 @@
       </c>
       <c r="R7" t="inlineStr">
         <is>
-          <t>-207.25320797397367</t>
+          <t>-207.2880356929771</t>
         </is>
       </c>
       <c r="S7" t="inlineStr">
@@ -1101,7 +1101,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>hh18</t>
+          <t>hh7</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -1121,7 +1121,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[17]</t>
+          <t>root.pop_gridConnections[6]</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -1131,7 +1131,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>0.252</t>
+          <t>0.3</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -1141,7 +1141,7 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>0.5020286982281488</t>
+          <t>0.602017313814645</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
@@ -1171,7 +1171,7 @@
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>-440.6174442320768</t>
+          <t>-475.6111135646337</t>
         </is>
       </c>
       <c r="Q8" t="inlineStr">
@@ -1181,7 +1181,7 @@
       </c>
       <c r="R8" t="inlineStr">
         <is>
-          <t>-207.25320797397367</t>
+          <t>-207.2880356929771</t>
         </is>
       </c>
       <c r="S8" t="inlineStr">
@@ -1196,12 +1196,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>com2</t>
+          <t>hh8</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>commercial</t>
+          <t>household</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -1216,7 +1216,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[19]</t>
+          <t>root.pop_gridConnections[7]</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -1226,7 +1226,7 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.3</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
@@ -1236,7 +1236,7 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.602017313814645</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
@@ -1266,7 +1266,7 @@
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-450.15911356463477</t>
         </is>
       </c>
       <c r="Q9" t="inlineStr">
@@ -1276,7 +1276,7 @@
       </c>
       <c r="R9" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-207.2880356929771</t>
         </is>
       </c>
       <c r="S9" t="inlineStr">
@@ -1291,7 +1291,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>hh17</t>
+          <t>hh9</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -1311,7 +1311,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[16]</t>
+          <t>root.pop_gridConnections[8]</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -1321,7 +1321,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>0.252</t>
+          <t>0.3</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -1331,7 +1331,7 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>0.5020286982281488</t>
+          <t>0.602017313814645</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
@@ -1361,7 +1361,7 @@
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>-280.05144423211055</t>
+          <t>-267.0391135646595</t>
         </is>
       </c>
       <c r="Q10" t="inlineStr">
@@ -1371,7 +1371,7 @@
       </c>
       <c r="R10" t="inlineStr">
         <is>
-          <t>-207.25320797397367</t>
+          <t>-207.2880356929771</t>
         </is>
       </c>
       <c r="S10" t="inlineStr">
@@ -1386,7 +1386,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>hh16</t>
+          <t>hh10</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -1396,37 +1396,37 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>sup1</t>
+          <t>hol1</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[0]</t>
+          <t>root.pop_energyHolons[0]( p_actorID = hol1, p_actorType = holon, p_parentActorID = sup2 )</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[15]</t>
+          <t>root.pop_gridConnections[9]</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>null</t>
+          <t>root.pop_energySuppliers[1]</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>0.252</t>
+          <t>0.3</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.5776933819433462</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>0.5020286982281488</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
@@ -1456,17 +1456,17 @@
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>-296.8934442321057</t>
+          <t>-377.75111356463697</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-397.82552304712624</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
         <is>
-          <t>-207.25320797397367</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="S11" t="inlineStr">
@@ -1481,12 +1481,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>com1</t>
+          <t>hh11</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>commercial</t>
+          <t>household</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -1501,7 +1501,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[18]</t>
+          <t>root.pop_gridConnections[10]</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -1511,12 +1511,12 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.3</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.5776933819433462</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
@@ -1551,12 +1551,12 @@
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-135.32711356467314</t>
         </is>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-397.82552304712624</t>
         </is>
       </c>
       <c r="R12" t="inlineStr">
@@ -1606,12 +1606,12 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>0.252</t>
+          <t>0.3</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>0.4817447104209508</t>
+          <t>0.5776933819433462</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
@@ -1646,12 +1646,12 @@
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>-374.13144423209104</t>
+          <t>-374.1811135646364</t>
         </is>
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>-397.75868197025045</t>
+          <t>-397.82552304712624</t>
         </is>
       </c>
       <c r="R13" t="inlineStr">
@@ -1671,7 +1671,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>hh3</t>
+          <t>hh13</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -1691,27 +1691,27 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[2]</t>
+          <t>root.pop_gridConnections[12]</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>null</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>0.252</t>
+          <t>0.3</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>0.4817447104209508</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.602017313814645</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
@@ -1741,17 +1741,17 @@
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>-163.6694442321168</t>
+          <t>-218.31911356466543</t>
         </is>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>-397.75868197025045</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="R14" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-207.2880356929771</t>
         </is>
       </c>
       <c r="S14" t="inlineStr">
@@ -1766,7 +1766,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>hh5</t>
+          <t>hh14</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -1786,7 +1786,7 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[4]</t>
+          <t>root.pop_gridConnections[13]</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -1796,7 +1796,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>0.252</t>
+          <t>0.3</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
@@ -1806,7 +1806,7 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>0.5020286982281488</t>
+          <t>0.602017313814645</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
@@ -1836,7 +1836,7 @@
       </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>-186.097444232117</t>
+          <t>-500.3491135646339</t>
         </is>
       </c>
       <c r="Q15" t="inlineStr">
@@ -1846,7 +1846,7 @@
       </c>
       <c r="R15" t="inlineStr">
         <is>
-          <t>-207.25320797397367</t>
+          <t>-207.2880356929771</t>
         </is>
       </c>
       <c r="S15" t="inlineStr">
@@ -1861,7 +1861,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>hh4</t>
+          <t>hh15</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1871,17 +1871,17 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>hol1</t>
+          <t>sup1</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>root.pop_energyHolons[0]( p_actorID = hol1, p_actorType = holon, p_parentActorID = sup2 )</t>
+          <t>root.pop_energySuppliers[0]</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[3]</t>
+          <t>root.pop_gridConnections[14]</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -1891,7 +1891,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>0.252</t>
+          <t>0.3</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
@@ -1901,7 +1901,7 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>0.5020286982281488</t>
+          <t>0.602017313814645</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
@@ -1931,7 +1931,7 @@
       </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>-797.4494442320381</t>
+          <t>-431.3431135646344</t>
         </is>
       </c>
       <c r="Q16" t="inlineStr">
@@ -1941,7 +1941,7 @@
       </c>
       <c r="R16" t="inlineStr">
         <is>
-          <t>-207.25320797397367</t>
+          <t>-207.2880356929771</t>
         </is>
       </c>
       <c r="S16" t="inlineStr">
@@ -1956,7 +1956,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>hh7</t>
+          <t>hh16</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1976,7 +1976,7 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[6]</t>
+          <t>root.pop_gridConnections[15]</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -1986,7 +1986,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>0.252</t>
+          <t>0.3</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
@@ -1996,7 +1996,7 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>0.5020286982281488</t>
+          <t>0.602017313814645</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
@@ -2026,7 +2026,7 @@
       </c>
       <c r="P17" t="inlineStr">
         <is>
-          <t>-475.5614442320712</t>
+          <t>-296.9431135646496</t>
         </is>
       </c>
       <c r="Q17" t="inlineStr">
@@ -2036,7 +2036,7 @@
       </c>
       <c r="R17" t="inlineStr">
         <is>
-          <t>-207.25320797397367</t>
+          <t>-207.2880356929771</t>
         </is>
       </c>
       <c r="S17" t="inlineStr">
@@ -2051,7 +2051,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>hh8</t>
+          <t>hh17</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -2071,7 +2071,7 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[7]</t>
+          <t>root.pop_gridConnections[16]</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -2081,7 +2081,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>0.252</t>
+          <t>0.3</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
@@ -2091,7 +2091,7 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>0.5020286982281488</t>
+          <t>0.602017313814645</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
@@ -2121,7 +2121,7 @@
       </c>
       <c r="P18" t="inlineStr">
         <is>
-          <t>-479.0474442320705</t>
+          <t>-280.1011135646563</t>
         </is>
       </c>
       <c r="Q18" t="inlineStr">
@@ -2131,7 +2131,7 @@
       </c>
       <c r="R18" t="inlineStr">
         <is>
-          <t>-207.25320797397367</t>
+          <t>-207.2880356929771</t>
         </is>
       </c>
       <c r="S18" t="inlineStr">
@@ -2146,7 +2146,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>hh9</t>
+          <t>hh18</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -2166,7 +2166,7 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[8]</t>
+          <t>root.pop_gridConnections[17]</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -2176,7 +2176,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>0.252</t>
+          <t>0.3</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
@@ -2186,7 +2186,7 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>0.5020286982281488</t>
+          <t>0.602017313814645</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
@@ -2216,7 +2216,7 @@
       </c>
       <c r="P19" t="inlineStr">
         <is>
-          <t>-266.9894442321134</t>
+          <t>-440.6671135646345</t>
         </is>
       </c>
       <c r="Q19" t="inlineStr">
@@ -2226,7 +2226,7 @@
       </c>
       <c r="R19" t="inlineStr">
         <is>
-          <t>-207.25320797397367</t>
+          <t>-207.2880356929771</t>
         </is>
       </c>
       <c r="S19" t="inlineStr">
@@ -2241,37 +2241,37 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>hh6</t>
+          <t>com1</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>household</t>
+          <t>commercial</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>sup1</t>
+          <t>hol1</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[0]</t>
+          <t>root.pop_energyHolons[0]( p_actorID = hol1, p_actorType = holon, p_parentActorID = sup2 )</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[5]</t>
+          <t>root.pop_gridConnections[18]</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>null</t>
+          <t>root.pop_energySuppliers[1]</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>0.252</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
@@ -2281,7 +2281,7 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>0.5020286982281488</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
@@ -2311,7 +2311,7 @@
       </c>
       <c r="P20" t="inlineStr">
         <is>
-          <t>-1164.781444232091</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="Q20" t="inlineStr">
@@ -2321,7 +2321,7 @@
       </c>
       <c r="R20" t="inlineStr">
         <is>
-          <t>-207.25320797397367</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="S20" t="inlineStr">
@@ -2336,42 +2336,42 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>hh10</t>
+          <t>com2</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>household</t>
+          <t>commercial</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>hol1</t>
+          <t>sup1</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>root.pop_energyHolons[0]( p_actorID = hol1, p_actorType = holon, p_parentActorID = sup2 )</t>
+          <t>root.pop_energySuppliers[0]</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[9]</t>
+          <t>root.pop_gridConnections[19]</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>null</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>0.252</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>0.4817447104209508</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
@@ -2406,12 +2406,12 @@
       </c>
       <c r="P21" t="inlineStr">
         <is>
-          <t>-377.70144423209103</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>-397.75868197025045</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="R21" t="inlineStr">

</xml_diff>